<commit_message>
* hide grid line * add comments to increase readability
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/application_for_leave.xlsx
+++ b/src/main/webapp/WEB-INF/books/application_for_leave.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D29A4C-13CB-0640-9166-46DAA38AACA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15" windowWidth="18015" windowHeight="9060"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="18020" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationForLeave" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
     <definedName name="To">ApplicationForLeave!$E$6</definedName>
     <definedName name="Total">ApplicationForLeave!$G$5</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -75,19 +81,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -96,7 +102,7 @@
       <u/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -414,6 +420,9 @@
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,9 +458,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,6 +465,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -505,7 +519,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,9 +551,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -571,6 +603,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -746,30 +796,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="2.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
     <col min="8" max="8" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="9" customHeight="1">
+    <row r="1" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="9" customHeight="1">
+    <row r="2" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
@@ -778,18 +828,18 @@
       <c r="G2" s="8"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="2:8" ht="25.5">
+    <row r="3" spans="2:8" ht="25" x14ac:dyDescent="0.2">
       <c r="B3" s="11"/>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" ht="21.75" customHeight="1">
+    <row r="4" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="11"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -802,66 +852,66 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="2:8" ht="24.75" customHeight="1">
+    <row r="5" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="17">
         <v>41306</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="25">
         <f>NETWORKDAYS(E5,E6)</f>
         <v>2</v>
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="2:8" ht="24" customHeight="1">
+    <row r="6" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
-      <c r="C6" s="23"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="17">
         <v>41309</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="25"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="2:8" ht="54.75" customHeight="1">
+    <row r="7" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="2:8" ht="35.25" customHeight="1">
+    <row r="8" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -870,18 +920,18 @@
       <c r="G9" s="5"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="2:8" ht="16.5" customHeight="1">
+    <row r="10" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -907,12 +957,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -920,12 +970,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>